<commit_message>
Clarified spreadsheet for the parts rack before sharing it with Rex.
</commit_message>
<xml_diff>
--- a/extrusion/parts_rack.xlsx
+++ b/extrusion/parts_rack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\scad\PrintableParts\half_baked\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\scad\PrintableParts\extrusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1067650D-498D-4EA4-B118-88FDD00AF68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB681D1-2609-4033-A3DF-F5EFE56787E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7474" yWindow="1234" windowWidth="19680" windowHeight="15069" xr2:uid="{D4F23621-1515-4DDC-BC07-15F8C63B856B}"/>
+    <workbookView xWindow="4457" yWindow="1963" windowWidth="15994" windowHeight="15068" xr2:uid="{D4F23621-1515-4DDC-BC07-15F8C63B856B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,6 +431,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">

</xml_diff>